<commit_message>
More work on excel export. Added coloration of section header.
</commit_message>
<xml_diff>
--- a/Template.xlsx
+++ b/Template.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Skill Building or Problem Solving</t>
   </si>
@@ -51,6 +51,18 @@
   </si>
   <si>
     <t>Taught and explained the different components/steps</t>
+  </si>
+  <si>
+    <t>Modeled the skill</t>
+  </si>
+  <si>
+    <t>&lt;- Each section has it's own header</t>
+  </si>
+  <si>
+    <t>&lt;- the skill is a larger font</t>
+  </si>
+  <si>
+    <t>&lt;- each selection is then listed under the skill</t>
   </si>
 </sst>
 </file>
@@ -392,15 +404,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -408,60 +420,74 @@
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
-    </row>
-    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A5" s="2" t="s">
+      <c r="H3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A9" s="2" t="s">
+    <row r="10" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-    </row>
-    <row r="10" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="A6:E6"/>
     <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A9:E9"/>
+    <mergeCell ref="A10:E10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Reworked the checkbox and labels into a single control. Excel export mostly functional
</commit_message>
<xml_diff>
--- a/Template.xlsx
+++ b/Template.xlsx
@@ -78,14 +78,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="18"/>
+      <b/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="14"/>
+      <b/>
+      <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -120,8 +122,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -407,7 +409,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>